<commit_message>
Add logic for sruveytitle and survey section
</commit_message>
<xml_diff>
--- a/app/routes/uploads/sec1_temp100.xlsx
+++ b/app/routes/uploads/sec1_temp100.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfred\Code\Mean\lakesidetrip\app\routes\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfred\Code\Mean\rawdata\app\routes\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3424" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="23">
   <si>
     <t>County</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Staff Training</t>
   </si>
   <si>
-    <t>SECTION 1</t>
-  </si>
-  <si>
     <t>IMCI</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
   </si>
   <si>
     <t>Trained in IMCI &amp; Still Working in CHU</t>
-  </si>
-  <si>
-    <t>FacilitiesSummary</t>
   </si>
 </sst>
 </file>
@@ -147,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,12 +157,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,16 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -219,10 +203,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH123"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -559,125 +548,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:34" s="6" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-    </row>
-    <row r="6" spans="1:34" s="8" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10" t="s">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10" t="s">
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10" t="s">
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,62 +650,62 @@
         <v>10</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="P7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="S7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="V7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="Y7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="AB7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -857,7 +795,7 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -947,7 +885,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1035,13 +973,13 @@
       <c r="AD10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
     </row>
     <row r="11" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1129,13 +1067,13 @@
       <c r="AD11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
     </row>
     <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1223,13 +1161,13 @@
       <c r="AD12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
     </row>
     <row r="13" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1317,13 +1255,13 @@
       <c r="AD13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
     </row>
     <row r="14" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1411,13 +1349,13 @@
       <c r="AD14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
     </row>
     <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1505,13 +1443,13 @@
       <c r="AD15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
     </row>
     <row r="16" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1599,13 +1537,13 @@
       <c r="AD16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
     </row>
     <row r="17" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1693,13 +1631,13 @@
       <c r="AD17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
     </row>
     <row r="18" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1787,13 +1725,13 @@
       <c r="AD18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
     </row>
     <row r="19" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1881,13 +1819,13 @@
       <c r="AD19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
-      <c r="AG19" s="11"/>
-      <c r="AH19" s="11"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
     </row>
     <row r="20" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1975,13 +1913,13 @@
       <c r="AD20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE20" s="11"/>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-      <c r="AH20" s="11"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
     </row>
     <row r="21" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2069,13 +2007,13 @@
       <c r="AD21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
     </row>
     <row r="22" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2163,13 +2101,13 @@
       <c r="AD22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
     </row>
     <row r="23" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
@@ -2257,13 +2195,13 @@
       <c r="AD23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
     </row>
     <row r="24" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
@@ -2351,13 +2289,13 @@
       <c r="AD24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
     </row>
     <row r="25" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>7</v>
       </c>
@@ -2445,13 +2383,13 @@
       <c r="AD25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE25" s="11"/>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11"/>
-      <c r="AH25" s="11"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="8"/>
     </row>
     <row r="26" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
@@ -2539,13 +2477,13 @@
       <c r="AD26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11"/>
-      <c r="AH26" s="11"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AH26" s="8"/>
     </row>
     <row r="27" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2633,13 +2571,13 @@
       <c r="AD27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8"/>
+      <c r="AH27" s="8"/>
     </row>
     <row r="28" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="2" t="s">
         <v>7</v>
       </c>
@@ -2727,13 +2665,13 @@
       <c r="AD28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE28" s="11"/>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-      <c r="AH28" s="11"/>
+      <c r="AE28" s="8"/>
+      <c r="AF28" s="8"/>
+      <c r="AG28" s="8"/>
+      <c r="AH28" s="8"/>
     </row>
     <row r="29" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
@@ -2821,13 +2759,13 @@
       <c r="AD29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE29" s="11"/>
-      <c r="AF29" s="11"/>
-      <c r="AG29" s="11"/>
-      <c r="AH29" s="11"/>
+      <c r="AE29" s="8"/>
+      <c r="AF29" s="8"/>
+      <c r="AG29" s="8"/>
+      <c r="AH29" s="8"/>
     </row>
     <row r="30" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -2915,13 +2853,13 @@
       <c r="AD30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE30" s="11"/>
-      <c r="AF30" s="11"/>
-      <c r="AG30" s="11"/>
-      <c r="AH30" s="11"/>
+      <c r="AE30" s="8"/>
+      <c r="AF30" s="8"/>
+      <c r="AG30" s="8"/>
+      <c r="AH30" s="8"/>
     </row>
     <row r="31" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
@@ -3009,13 +2947,13 @@
       <c r="AD31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="11"/>
-      <c r="AG31" s="11"/>
-      <c r="AH31" s="11"/>
+      <c r="AE31" s="8"/>
+      <c r="AF31" s="8"/>
+      <c r="AG31" s="8"/>
+      <c r="AH31" s="8"/>
     </row>
     <row r="32" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
@@ -3103,13 +3041,13 @@
       <c r="AD32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-      <c r="AH32" s="11"/>
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="8"/>
+      <c r="AG32" s="8"/>
+      <c r="AH32" s="8"/>
     </row>
     <row r="33" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
         <v>7</v>
       </c>
@@ -3197,13 +3135,13 @@
       <c r="AD33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
-      <c r="AG33" s="11"/>
-      <c r="AH33" s="11"/>
+      <c r="AE33" s="8"/>
+      <c r="AF33" s="8"/>
+      <c r="AG33" s="8"/>
+      <c r="AH33" s="8"/>
     </row>
     <row r="34" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
         <v>7</v>
       </c>
@@ -3291,13 +3229,13 @@
       <c r="AD34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE34" s="11"/>
-      <c r="AF34" s="11"/>
-      <c r="AG34" s="11"/>
-      <c r="AH34" s="11"/>
+      <c r="AE34" s="8"/>
+      <c r="AF34" s="8"/>
+      <c r="AG34" s="8"/>
+      <c r="AH34" s="8"/>
     </row>
     <row r="35" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
@@ -3385,13 +3323,13 @@
       <c r="AD35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="11"/>
-      <c r="AG35" s="11"/>
-      <c r="AH35" s="11"/>
+      <c r="AE35" s="8"/>
+      <c r="AF35" s="8"/>
+      <c r="AG35" s="8"/>
+      <c r="AH35" s="8"/>
     </row>
     <row r="36" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
@@ -3479,13 +3417,13 @@
       <c r="AD36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
-      <c r="AG36" s="11"/>
-      <c r="AH36" s="11"/>
+      <c r="AE36" s="8"/>
+      <c r="AF36" s="8"/>
+      <c r="AG36" s="8"/>
+      <c r="AH36" s="8"/>
     </row>
     <row r="37" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
         <v>7</v>
       </c>
@@ -3573,13 +3511,13 @@
       <c r="AD37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
-      <c r="AG37" s="11"/>
-      <c r="AH37" s="11"/>
+      <c r="AE37" s="8"/>
+      <c r="AF37" s="8"/>
+      <c r="AG37" s="8"/>
+      <c r="AH37" s="8"/>
     </row>
     <row r="38" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
@@ -3667,13 +3605,13 @@
       <c r="AD38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="11"/>
-      <c r="AG38" s="11"/>
-      <c r="AH38" s="11"/>
+      <c r="AE38" s="8"/>
+      <c r="AF38" s="8"/>
+      <c r="AG38" s="8"/>
+      <c r="AH38" s="8"/>
     </row>
     <row r="39" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
         <v>7</v>
       </c>
@@ -3761,13 +3699,13 @@
       <c r="AD39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE39" s="11"/>
-      <c r="AF39" s="11"/>
-      <c r="AG39" s="11"/>
-      <c r="AH39" s="11"/>
+      <c r="AE39" s="8"/>
+      <c r="AF39" s="8"/>
+      <c r="AG39" s="8"/>
+      <c r="AH39" s="8"/>
     </row>
     <row r="40" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
         <v>7</v>
       </c>
@@ -3855,13 +3793,13 @@
       <c r="AD40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE40" s="11"/>
-      <c r="AF40" s="11"/>
-      <c r="AG40" s="11"/>
-      <c r="AH40" s="11"/>
+      <c r="AE40" s="8"/>
+      <c r="AF40" s="8"/>
+      <c r="AG40" s="8"/>
+      <c r="AH40" s="8"/>
     </row>
     <row r="41" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -3949,13 +3887,13 @@
       <c r="AD41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE41" s="11"/>
-      <c r="AF41" s="11"/>
-      <c r="AG41" s="11"/>
-      <c r="AH41" s="11"/>
+      <c r="AE41" s="8"/>
+      <c r="AF41" s="8"/>
+      <c r="AG41" s="8"/>
+      <c r="AH41" s="8"/>
     </row>
     <row r="42" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="2" t="s">
         <v>7</v>
       </c>
@@ -4043,13 +3981,13 @@
       <c r="AD42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE42" s="11"/>
-      <c r="AF42" s="11"/>
-      <c r="AG42" s="11"/>
-      <c r="AH42" s="11"/>
+      <c r="AE42" s="8"/>
+      <c r="AF42" s="8"/>
+      <c r="AG42" s="8"/>
+      <c r="AH42" s="8"/>
     </row>
     <row r="43" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="2" t="s">
         <v>7</v>
       </c>
@@ -4137,13 +4075,13 @@
       <c r="AD43" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE43" s="11"/>
-      <c r="AF43" s="11"/>
-      <c r="AG43" s="11"/>
-      <c r="AH43" s="11"/>
+      <c r="AE43" s="8"/>
+      <c r="AF43" s="8"/>
+      <c r="AG43" s="8"/>
+      <c r="AH43" s="8"/>
     </row>
     <row r="44" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
@@ -4231,13 +4169,13 @@
       <c r="AD44" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE44" s="11"/>
-      <c r="AF44" s="11"/>
-      <c r="AG44" s="11"/>
-      <c r="AH44" s="11"/>
+      <c r="AE44" s="8"/>
+      <c r="AF44" s="8"/>
+      <c r="AG44" s="8"/>
+      <c r="AH44" s="8"/>
     </row>
     <row r="45" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="8"/>
       <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
@@ -4325,13 +4263,13 @@
       <c r="AD45" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE45" s="11"/>
-      <c r="AF45" s="11"/>
-      <c r="AG45" s="11"/>
-      <c r="AH45" s="11"/>
+      <c r="AE45" s="8"/>
+      <c r="AF45" s="8"/>
+      <c r="AG45" s="8"/>
+      <c r="AH45" s="8"/>
     </row>
     <row r="46" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="8"/>
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
@@ -4419,13 +4357,13 @@
       <c r="AD46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE46" s="11"/>
-      <c r="AF46" s="11"/>
-      <c r="AG46" s="11"/>
-      <c r="AH46" s="11"/>
+      <c r="AE46" s="8"/>
+      <c r="AF46" s="8"/>
+      <c r="AG46" s="8"/>
+      <c r="AH46" s="8"/>
     </row>
     <row r="47" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
@@ -4513,13 +4451,13 @@
       <c r="AD47" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE47" s="11"/>
-      <c r="AF47" s="11"/>
-      <c r="AG47" s="11"/>
-      <c r="AH47" s="11"/>
+      <c r="AE47" s="8"/>
+      <c r="AF47" s="8"/>
+      <c r="AG47" s="8"/>
+      <c r="AH47" s="8"/>
     </row>
     <row r="48" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+      <c r="A48" s="8"/>
       <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
@@ -4607,13 +4545,13 @@
       <c r="AD48" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE48" s="11"/>
-      <c r="AF48" s="11"/>
-      <c r="AG48" s="11"/>
-      <c r="AH48" s="11"/>
+      <c r="AE48" s="8"/>
+      <c r="AF48" s="8"/>
+      <c r="AG48" s="8"/>
+      <c r="AH48" s="8"/>
     </row>
     <row r="49" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
@@ -4701,13 +4639,13 @@
       <c r="AD49" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE49" s="11"/>
-      <c r="AF49" s="11"/>
-      <c r="AG49" s="11"/>
-      <c r="AH49" s="11"/>
+      <c r="AE49" s="8"/>
+      <c r="AF49" s="8"/>
+      <c r="AG49" s="8"/>
+      <c r="AH49" s="8"/>
     </row>
     <row r="50" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4795,13 +4733,13 @@
       <c r="AD50" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE50" s="11"/>
-      <c r="AF50" s="11"/>
-      <c r="AG50" s="11"/>
-      <c r="AH50" s="11"/>
+      <c r="AE50" s="8"/>
+      <c r="AF50" s="8"/>
+      <c r="AG50" s="8"/>
+      <c r="AH50" s="8"/>
     </row>
     <row r="51" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
@@ -4889,13 +4827,13 @@
       <c r="AD51" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE51" s="11"/>
-      <c r="AF51" s="11"/>
-      <c r="AG51" s="11"/>
-      <c r="AH51" s="11"/>
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="8"/>
+      <c r="AG51" s="8"/>
+      <c r="AH51" s="8"/>
     </row>
     <row r="52" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="2" t="s">
         <v>7</v>
       </c>
@@ -4983,13 +4921,13 @@
       <c r="AD52" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE52" s="11"/>
-      <c r="AF52" s="11"/>
-      <c r="AG52" s="11"/>
-      <c r="AH52" s="11"/>
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="8"/>
+      <c r="AG52" s="8"/>
+      <c r="AH52" s="8"/>
     </row>
     <row r="53" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
@@ -5077,13 +5015,13 @@
       <c r="AD53" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE53" s="11"/>
-      <c r="AF53" s="11"/>
-      <c r="AG53" s="11"/>
-      <c r="AH53" s="11"/>
+      <c r="AE53" s="8"/>
+      <c r="AF53" s="8"/>
+      <c r="AG53" s="8"/>
+      <c r="AH53" s="8"/>
     </row>
     <row r="54" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
@@ -5171,13 +5109,13 @@
       <c r="AD54" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE54" s="11"/>
-      <c r="AF54" s="11"/>
-      <c r="AG54" s="11"/>
-      <c r="AH54" s="11"/>
+      <c r="AE54" s="8"/>
+      <c r="AF54" s="8"/>
+      <c r="AG54" s="8"/>
+      <c r="AH54" s="8"/>
     </row>
     <row r="55" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+      <c r="A55" s="8"/>
       <c r="B55" s="2" t="s">
         <v>7</v>
       </c>
@@ -5265,13 +5203,13 @@
       <c r="AD55" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE55" s="11"/>
-      <c r="AF55" s="11"/>
-      <c r="AG55" s="11"/>
-      <c r="AH55" s="11"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="8"/>
+      <c r="AG55" s="8"/>
+      <c r="AH55" s="8"/>
     </row>
     <row r="56" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="2" t="s">
         <v>7</v>
       </c>
@@ -5359,13 +5297,13 @@
       <c r="AD56" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE56" s="11"/>
-      <c r="AF56" s="11"/>
-      <c r="AG56" s="11"/>
-      <c r="AH56" s="11"/>
+      <c r="AE56" s="8"/>
+      <c r="AF56" s="8"/>
+      <c r="AG56" s="8"/>
+      <c r="AH56" s="8"/>
     </row>
     <row r="57" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
+      <c r="A57" s="8"/>
       <c r="B57" s="2" t="s">
         <v>7</v>
       </c>
@@ -5453,13 +5391,13 @@
       <c r="AD57" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE57" s="11"/>
-      <c r="AF57" s="11"/>
-      <c r="AG57" s="11"/>
-      <c r="AH57" s="11"/>
+      <c r="AE57" s="8"/>
+      <c r="AF57" s="8"/>
+      <c r="AG57" s="8"/>
+      <c r="AH57" s="8"/>
     </row>
     <row r="58" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="2" t="s">
         <v>7</v>
       </c>
@@ -5547,13 +5485,13 @@
       <c r="AD58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE58" s="11"/>
-      <c r="AF58" s="11"/>
-      <c r="AG58" s="11"/>
-      <c r="AH58" s="11"/>
+      <c r="AE58" s="8"/>
+      <c r="AF58" s="8"/>
+      <c r="AG58" s="8"/>
+      <c r="AH58" s="8"/>
     </row>
     <row r="59" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="2" t="s">
         <v>7</v>
       </c>
@@ -5641,13 +5579,13 @@
       <c r="AD59" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE59" s="11"/>
-      <c r="AF59" s="11"/>
-      <c r="AG59" s="11"/>
-      <c r="AH59" s="11"/>
+      <c r="AE59" s="8"/>
+      <c r="AF59" s="8"/>
+      <c r="AG59" s="8"/>
+      <c r="AH59" s="8"/>
     </row>
     <row r="60" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="2" t="s">
         <v>7</v>
       </c>
@@ -5735,13 +5673,13 @@
       <c r="AD60" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE60" s="11"/>
-      <c r="AF60" s="11"/>
-      <c r="AG60" s="11"/>
-      <c r="AH60" s="11"/>
+      <c r="AE60" s="8"/>
+      <c r="AF60" s="8"/>
+      <c r="AG60" s="8"/>
+      <c r="AH60" s="8"/>
     </row>
     <row r="61" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="2" t="s">
         <v>7</v>
       </c>
@@ -5829,13 +5767,13 @@
       <c r="AD61" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE61" s="11"/>
-      <c r="AF61" s="11"/>
-      <c r="AG61" s="11"/>
-      <c r="AH61" s="11"/>
+      <c r="AE61" s="8"/>
+      <c r="AF61" s="8"/>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="8"/>
     </row>
     <row r="62" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="2" t="s">
         <v>7</v>
       </c>
@@ -5923,13 +5861,13 @@
       <c r="AD62" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE62" s="11"/>
-      <c r="AF62" s="11"/>
-      <c r="AG62" s="11"/>
-      <c r="AH62" s="11"/>
+      <c r="AE62" s="8"/>
+      <c r="AF62" s="8"/>
+      <c r="AG62" s="8"/>
+      <c r="AH62" s="8"/>
     </row>
     <row r="63" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="2" t="s">
         <v>7</v>
       </c>
@@ -6017,13 +5955,13 @@
       <c r="AD63" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE63" s="11"/>
-      <c r="AF63" s="11"/>
-      <c r="AG63" s="11"/>
-      <c r="AH63" s="11"/>
+      <c r="AE63" s="8"/>
+      <c r="AF63" s="8"/>
+      <c r="AG63" s="8"/>
+      <c r="AH63" s="8"/>
     </row>
     <row r="64" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
+      <c r="A64" s="8"/>
       <c r="B64" s="2" t="s">
         <v>7</v>
       </c>
@@ -6111,13 +6049,13 @@
       <c r="AD64" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE64" s="11"/>
-      <c r="AF64" s="11"/>
-      <c r="AG64" s="11"/>
-      <c r="AH64" s="11"/>
+      <c r="AE64" s="8"/>
+      <c r="AF64" s="8"/>
+      <c r="AG64" s="8"/>
+      <c r="AH64" s="8"/>
     </row>
     <row r="65" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
+      <c r="A65" s="8"/>
       <c r="B65" s="2" t="s">
         <v>7</v>
       </c>
@@ -6205,13 +6143,13 @@
       <c r="AD65" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE65" s="11"/>
-      <c r="AF65" s="11"/>
-      <c r="AG65" s="11"/>
-      <c r="AH65" s="11"/>
+      <c r="AE65" s="8"/>
+      <c r="AF65" s="8"/>
+      <c r="AG65" s="8"/>
+      <c r="AH65" s="8"/>
     </row>
     <row r="66" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
+      <c r="A66" s="8"/>
       <c r="B66" s="2" t="s">
         <v>7</v>
       </c>
@@ -6299,13 +6237,13 @@
       <c r="AD66" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE66" s="11"/>
-      <c r="AF66" s="11"/>
-      <c r="AG66" s="11"/>
-      <c r="AH66" s="11"/>
+      <c r="AE66" s="8"/>
+      <c r="AF66" s="8"/>
+      <c r="AG66" s="8"/>
+      <c r="AH66" s="8"/>
     </row>
     <row r="67" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -6393,13 +6331,13 @@
       <c r="AD67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE67" s="11"/>
-      <c r="AF67" s="11"/>
-      <c r="AG67" s="11"/>
-      <c r="AH67" s="11"/>
+      <c r="AE67" s="8"/>
+      <c r="AF67" s="8"/>
+      <c r="AG67" s="8"/>
+      <c r="AH67" s="8"/>
     </row>
     <row r="68" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="2" t="s">
         <v>7</v>
       </c>
@@ -6487,13 +6425,13 @@
       <c r="AD68" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE68" s="11"/>
-      <c r="AF68" s="11"/>
-      <c r="AG68" s="11"/>
-      <c r="AH68" s="11"/>
+      <c r="AE68" s="8"/>
+      <c r="AF68" s="8"/>
+      <c r="AG68" s="8"/>
+      <c r="AH68" s="8"/>
     </row>
     <row r="69" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="2" t="s">
         <v>7</v>
       </c>
@@ -6581,13 +6519,13 @@
       <c r="AD69" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE69" s="11"/>
-      <c r="AF69" s="11"/>
-      <c r="AG69" s="11"/>
-      <c r="AH69" s="11"/>
+      <c r="AE69" s="8"/>
+      <c r="AF69" s="8"/>
+      <c r="AG69" s="8"/>
+      <c r="AH69" s="8"/>
     </row>
     <row r="70" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="2" t="s">
         <v>7</v>
       </c>
@@ -6675,13 +6613,13 @@
       <c r="AD70" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE70" s="11"/>
-      <c r="AF70" s="11"/>
-      <c r="AG70" s="11"/>
-      <c r="AH70" s="11"/>
+      <c r="AE70" s="8"/>
+      <c r="AF70" s="8"/>
+      <c r="AG70" s="8"/>
+      <c r="AH70" s="8"/>
     </row>
     <row r="71" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="2" t="s">
         <v>7</v>
       </c>
@@ -6769,13 +6707,13 @@
       <c r="AD71" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE71" s="11"/>
-      <c r="AF71" s="11"/>
-      <c r="AG71" s="11"/>
-      <c r="AH71" s="11"/>
+      <c r="AE71" s="8"/>
+      <c r="AF71" s="8"/>
+      <c r="AG71" s="8"/>
+      <c r="AH71" s="8"/>
     </row>
     <row r="72" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="2" t="s">
         <v>7</v>
       </c>
@@ -6863,13 +6801,13 @@
       <c r="AD72" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE72" s="11"/>
-      <c r="AF72" s="11"/>
-      <c r="AG72" s="11"/>
-      <c r="AH72" s="11"/>
+      <c r="AE72" s="8"/>
+      <c r="AF72" s="8"/>
+      <c r="AG72" s="8"/>
+      <c r="AH72" s="8"/>
     </row>
     <row r="73" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
+      <c r="A73" s="8"/>
       <c r="B73" s="2" t="s">
         <v>7</v>
       </c>
@@ -6957,13 +6895,13 @@
       <c r="AD73" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE73" s="11"/>
-      <c r="AF73" s="11"/>
-      <c r="AG73" s="11"/>
-      <c r="AH73" s="11"/>
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="8"/>
+      <c r="AH73" s="8"/>
     </row>
     <row r="74" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="2" t="s">
         <v>7</v>
       </c>
@@ -7051,13 +6989,13 @@
       <c r="AD74" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE74" s="11"/>
-      <c r="AF74" s="11"/>
-      <c r="AG74" s="11"/>
-      <c r="AH74" s="11"/>
+      <c r="AE74" s="8"/>
+      <c r="AF74" s="8"/>
+      <c r="AG74" s="8"/>
+      <c r="AH74" s="8"/>
     </row>
     <row r="75" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
+      <c r="A75" s="8"/>
       <c r="B75" s="2" t="s">
         <v>7</v>
       </c>
@@ -7145,13 +7083,13 @@
       <c r="AD75" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE75" s="11"/>
-      <c r="AF75" s="11"/>
-      <c r="AG75" s="11"/>
-      <c r="AH75" s="11"/>
+      <c r="AE75" s="8"/>
+      <c r="AF75" s="8"/>
+      <c r="AG75" s="8"/>
+      <c r="AH75" s="8"/>
     </row>
     <row r="76" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+      <c r="A76" s="8"/>
       <c r="B76" s="2" t="s">
         <v>7</v>
       </c>
@@ -7239,13 +7177,13 @@
       <c r="AD76" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE76" s="11"/>
-      <c r="AF76" s="11"/>
-      <c r="AG76" s="11"/>
-      <c r="AH76" s="11"/>
+      <c r="AE76" s="8"/>
+      <c r="AF76" s="8"/>
+      <c r="AG76" s="8"/>
+      <c r="AH76" s="8"/>
     </row>
     <row r="77" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="2" t="s">
         <v>7</v>
       </c>
@@ -7333,13 +7271,13 @@
       <c r="AD77" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE77" s="11"/>
-      <c r="AF77" s="11"/>
-      <c r="AG77" s="11"/>
-      <c r="AH77" s="11"/>
+      <c r="AE77" s="8"/>
+      <c r="AF77" s="8"/>
+      <c r="AG77" s="8"/>
+      <c r="AH77" s="8"/>
     </row>
     <row r="78" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="2" t="s">
         <v>7</v>
       </c>
@@ -7427,13 +7365,13 @@
       <c r="AD78" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE78" s="11"/>
-      <c r="AF78" s="11"/>
-      <c r="AG78" s="11"/>
-      <c r="AH78" s="11"/>
+      <c r="AE78" s="8"/>
+      <c r="AF78" s="8"/>
+      <c r="AG78" s="8"/>
+      <c r="AH78" s="8"/>
     </row>
     <row r="79" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="2" t="s">
         <v>7</v>
       </c>
@@ -7521,13 +7459,13 @@
       <c r="AD79" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE79" s="11"/>
-      <c r="AF79" s="11"/>
-      <c r="AG79" s="11"/>
-      <c r="AH79" s="11"/>
+      <c r="AE79" s="8"/>
+      <c r="AF79" s="8"/>
+      <c r="AG79" s="8"/>
+      <c r="AH79" s="8"/>
     </row>
     <row r="80" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="2" t="s">
         <v>7</v>
       </c>
@@ -7615,13 +7553,13 @@
       <c r="AD80" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE80" s="11"/>
-      <c r="AF80" s="11"/>
-      <c r="AG80" s="11"/>
-      <c r="AH80" s="11"/>
+      <c r="AE80" s="8"/>
+      <c r="AF80" s="8"/>
+      <c r="AG80" s="8"/>
+      <c r="AH80" s="8"/>
     </row>
     <row r="81" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="2" t="s">
         <v>7</v>
       </c>
@@ -7709,13 +7647,13 @@
       <c r="AD81" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE81" s="11"/>
-      <c r="AF81" s="11"/>
-      <c r="AG81" s="11"/>
-      <c r="AH81" s="11"/>
+      <c r="AE81" s="8"/>
+      <c r="AF81" s="8"/>
+      <c r="AG81" s="8"/>
+      <c r="AH81" s="8"/>
     </row>
     <row r="82" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="2" t="s">
         <v>7</v>
       </c>
@@ -7803,13 +7741,13 @@
       <c r="AD82" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE82" s="11"/>
-      <c r="AF82" s="11"/>
-      <c r="AG82" s="11"/>
-      <c r="AH82" s="11"/>
+      <c r="AE82" s="8"/>
+      <c r="AF82" s="8"/>
+      <c r="AG82" s="8"/>
+      <c r="AH82" s="8"/>
     </row>
     <row r="83" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="8"/>
       <c r="B83" s="2" t="s">
         <v>7</v>
       </c>
@@ -7897,13 +7835,13 @@
       <c r="AD83" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE83" s="11"/>
-      <c r="AF83" s="11"/>
-      <c r="AG83" s="11"/>
-      <c r="AH83" s="11"/>
+      <c r="AE83" s="8"/>
+      <c r="AF83" s="8"/>
+      <c r="AG83" s="8"/>
+      <c r="AH83" s="8"/>
     </row>
     <row r="84" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+      <c r="A84" s="8"/>
       <c r="B84" s="2" t="s">
         <v>7</v>
       </c>
@@ -7991,13 +7929,13 @@
       <c r="AD84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE84" s="11"/>
-      <c r="AF84" s="11"/>
-      <c r="AG84" s="11"/>
-      <c r="AH84" s="11"/>
+      <c r="AE84" s="8"/>
+      <c r="AF84" s="8"/>
+      <c r="AG84" s="8"/>
+      <c r="AH84" s="8"/>
     </row>
     <row r="85" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+      <c r="A85" s="8"/>
       <c r="B85" s="2" t="s">
         <v>7</v>
       </c>
@@ -8085,13 +8023,13 @@
       <c r="AD85" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE85" s="11"/>
-      <c r="AF85" s="11"/>
-      <c r="AG85" s="11"/>
-      <c r="AH85" s="11"/>
+      <c r="AE85" s="8"/>
+      <c r="AF85" s="8"/>
+      <c r="AG85" s="8"/>
+      <c r="AH85" s="8"/>
     </row>
     <row r="86" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
+      <c r="A86" s="8"/>
       <c r="B86" s="2" t="s">
         <v>7</v>
       </c>
@@ -8179,13 +8117,13 @@
       <c r="AD86" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE86" s="11"/>
-      <c r="AF86" s="11"/>
-      <c r="AG86" s="11"/>
-      <c r="AH86" s="11"/>
+      <c r="AE86" s="8"/>
+      <c r="AF86" s="8"/>
+      <c r="AG86" s="8"/>
+      <c r="AH86" s="8"/>
     </row>
     <row r="87" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+      <c r="A87" s="8"/>
       <c r="B87" s="2" t="s">
         <v>7</v>
       </c>
@@ -8273,13 +8211,13 @@
       <c r="AD87" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE87" s="11"/>
-      <c r="AF87" s="11"/>
-      <c r="AG87" s="11"/>
-      <c r="AH87" s="11"/>
+      <c r="AE87" s="8"/>
+      <c r="AF87" s="8"/>
+      <c r="AG87" s="8"/>
+      <c r="AH87" s="8"/>
     </row>
     <row r="88" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="2" t="s">
         <v>7</v>
       </c>
@@ -8367,13 +8305,13 @@
       <c r="AD88" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE88" s="11"/>
-      <c r="AF88" s="11"/>
-      <c r="AG88" s="11"/>
-      <c r="AH88" s="11"/>
+      <c r="AE88" s="8"/>
+      <c r="AF88" s="8"/>
+      <c r="AG88" s="8"/>
+      <c r="AH88" s="8"/>
     </row>
     <row r="89" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
@@ -8461,13 +8399,13 @@
       <c r="AD89" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE89" s="11"/>
-      <c r="AF89" s="11"/>
-      <c r="AG89" s="11"/>
-      <c r="AH89" s="11"/>
+      <c r="AE89" s="8"/>
+      <c r="AF89" s="8"/>
+      <c r="AG89" s="8"/>
+      <c r="AH89" s="8"/>
     </row>
     <row r="90" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
+      <c r="A90" s="8"/>
       <c r="B90" s="2" t="s">
         <v>7</v>
       </c>
@@ -8555,13 +8493,13 @@
       <c r="AD90" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE90" s="11"/>
-      <c r="AF90" s="11"/>
-      <c r="AG90" s="11"/>
-      <c r="AH90" s="11"/>
+      <c r="AE90" s="8"/>
+      <c r="AF90" s="8"/>
+      <c r="AG90" s="8"/>
+      <c r="AH90" s="8"/>
     </row>
     <row r="91" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="2" t="s">
         <v>7</v>
       </c>
@@ -8649,13 +8587,13 @@
       <c r="AD91" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE91" s="11"/>
-      <c r="AF91" s="11"/>
-      <c r="AG91" s="11"/>
-      <c r="AH91" s="11"/>
+      <c r="AE91" s="8"/>
+      <c r="AF91" s="8"/>
+      <c r="AG91" s="8"/>
+      <c r="AH91" s="8"/>
     </row>
     <row r="92" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="11"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="2" t="s">
         <v>7</v>
       </c>
@@ -8743,13 +8681,13 @@
       <c r="AD92" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE92" s="11"/>
-      <c r="AF92" s="11"/>
-      <c r="AG92" s="11"/>
-      <c r="AH92" s="11"/>
+      <c r="AE92" s="8"/>
+      <c r="AF92" s="8"/>
+      <c r="AG92" s="8"/>
+      <c r="AH92" s="8"/>
     </row>
     <row r="93" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="11"/>
+      <c r="A93" s="8"/>
       <c r="B93" s="2" t="s">
         <v>7</v>
       </c>
@@ -8837,13 +8775,13 @@
       <c r="AD93" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE93" s="11"/>
-      <c r="AF93" s="11"/>
-      <c r="AG93" s="11"/>
-      <c r="AH93" s="11"/>
+      <c r="AE93" s="8"/>
+      <c r="AF93" s="8"/>
+      <c r="AG93" s="8"/>
+      <c r="AH93" s="8"/>
     </row>
     <row r="94" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="11"/>
+      <c r="A94" s="8"/>
       <c r="B94" s="2" t="s">
         <v>7</v>
       </c>
@@ -8931,13 +8869,13 @@
       <c r="AD94" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE94" s="11"/>
-      <c r="AF94" s="11"/>
-      <c r="AG94" s="11"/>
-      <c r="AH94" s="11"/>
+      <c r="AE94" s="8"/>
+      <c r="AF94" s="8"/>
+      <c r="AG94" s="8"/>
+      <c r="AH94" s="8"/>
     </row>
     <row r="95" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
+      <c r="A95" s="8"/>
       <c r="B95" s="2" t="s">
         <v>7</v>
       </c>
@@ -9025,13 +8963,13 @@
       <c r="AD95" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE95" s="11"/>
-      <c r="AF95" s="11"/>
-      <c r="AG95" s="11"/>
-      <c r="AH95" s="11"/>
+      <c r="AE95" s="8"/>
+      <c r="AF95" s="8"/>
+      <c r="AG95" s="8"/>
+      <c r="AH95" s="8"/>
     </row>
     <row r="96" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
+      <c r="A96" s="8"/>
       <c r="B96" s="2" t="s">
         <v>7</v>
       </c>
@@ -9119,13 +9057,13 @@
       <c r="AD96" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE96" s="11"/>
-      <c r="AF96" s="11"/>
-      <c r="AG96" s="11"/>
-      <c r="AH96" s="11"/>
+      <c r="AE96" s="8"/>
+      <c r="AF96" s="8"/>
+      <c r="AG96" s="8"/>
+      <c r="AH96" s="8"/>
     </row>
     <row r="97" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="11"/>
+      <c r="A97" s="8"/>
       <c r="B97" s="2" t="s">
         <v>7</v>
       </c>
@@ -9213,13 +9151,13 @@
       <c r="AD97" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE97" s="11"/>
-      <c r="AF97" s="11"/>
-      <c r="AG97" s="11"/>
-      <c r="AH97" s="11"/>
+      <c r="AE97" s="8"/>
+      <c r="AF97" s="8"/>
+      <c r="AG97" s="8"/>
+      <c r="AH97" s="8"/>
     </row>
     <row r="98" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
+      <c r="A98" s="8"/>
       <c r="B98" s="2" t="s">
         <v>7</v>
       </c>
@@ -9307,13 +9245,13 @@
       <c r="AD98" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE98" s="11"/>
-      <c r="AF98" s="11"/>
-      <c r="AG98" s="11"/>
-      <c r="AH98" s="11"/>
+      <c r="AE98" s="8"/>
+      <c r="AF98" s="8"/>
+      <c r="AG98" s="8"/>
+      <c r="AH98" s="8"/>
     </row>
     <row r="99" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
+      <c r="A99" s="8"/>
       <c r="B99" s="2" t="s">
         <v>7</v>
       </c>
@@ -9401,13 +9339,13 @@
       <c r="AD99" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE99" s="11"/>
-      <c r="AF99" s="11"/>
-      <c r="AG99" s="11"/>
-      <c r="AH99" s="11"/>
+      <c r="AE99" s="8"/>
+      <c r="AF99" s="8"/>
+      <c r="AG99" s="8"/>
+      <c r="AH99" s="8"/>
     </row>
     <row r="100" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="11"/>
+      <c r="A100" s="8"/>
       <c r="B100" s="2" t="s">
         <v>7</v>
       </c>
@@ -9495,13 +9433,13 @@
       <c r="AD100" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE100" s="11"/>
-      <c r="AF100" s="11"/>
-      <c r="AG100" s="11"/>
-      <c r="AH100" s="11"/>
+      <c r="AE100" s="8"/>
+      <c r="AF100" s="8"/>
+      <c r="AG100" s="8"/>
+      <c r="AH100" s="8"/>
     </row>
     <row r="101" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
+      <c r="A101" s="8"/>
       <c r="B101" s="2" t="s">
         <v>7</v>
       </c>
@@ -9589,13 +9527,13 @@
       <c r="AD101" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE101" s="11"/>
-      <c r="AF101" s="11"/>
-      <c r="AG101" s="11"/>
-      <c r="AH101" s="11"/>
+      <c r="AE101" s="8"/>
+      <c r="AF101" s="8"/>
+      <c r="AG101" s="8"/>
+      <c r="AH101" s="8"/>
     </row>
     <row r="102" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
+      <c r="A102" s="8"/>
       <c r="B102" s="2" t="s">
         <v>7</v>
       </c>
@@ -9683,10 +9621,10 @@
       <c r="AD102" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE102" s="11"/>
-      <c r="AF102" s="11"/>
-      <c r="AG102" s="11"/>
-      <c r="AH102" s="11"/>
+      <c r="AE102" s="8"/>
+      <c r="AF102" s="8"/>
+      <c r="AG102" s="8"/>
+      <c r="AH102" s="8"/>
     </row>
     <row r="103" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
@@ -9776,10 +9714,10 @@
       <c r="AD103" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE103" s="11"/>
-      <c r="AF103" s="11"/>
-      <c r="AG103" s="11"/>
-      <c r="AH103" s="11"/>
+      <c r="AE103" s="8"/>
+      <c r="AF103" s="8"/>
+      <c r="AG103" s="8"/>
+      <c r="AH103" s="8"/>
     </row>
     <row r="104" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
@@ -9869,10 +9807,10 @@
       <c r="AD104" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE104" s="11"/>
-      <c r="AF104" s="11"/>
-      <c r="AG104" s="11"/>
-      <c r="AH104" s="11"/>
+      <c r="AE104" s="8"/>
+      <c r="AF104" s="8"/>
+      <c r="AG104" s="8"/>
+      <c r="AH104" s="8"/>
     </row>
     <row r="105" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
@@ -9962,10 +9900,10 @@
       <c r="AD105" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE105" s="11"/>
-      <c r="AF105" s="11"/>
-      <c r="AG105" s="11"/>
-      <c r="AH105" s="11"/>
+      <c r="AE105" s="8"/>
+      <c r="AF105" s="8"/>
+      <c r="AG105" s="8"/>
+      <c r="AH105" s="8"/>
     </row>
     <row r="106" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
@@ -10055,10 +9993,10 @@
       <c r="AD106" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE106" s="11"/>
-      <c r="AF106" s="11"/>
-      <c r="AG106" s="11"/>
-      <c r="AH106" s="11"/>
+      <c r="AE106" s="8"/>
+      <c r="AF106" s="8"/>
+      <c r="AG106" s="8"/>
+      <c r="AH106" s="8"/>
     </row>
     <row r="107" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
@@ -10148,10 +10086,10 @@
       <c r="AD107" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE107" s="11"/>
-      <c r="AF107" s="11"/>
-      <c r="AG107" s="11"/>
-      <c r="AH107" s="11"/>
+      <c r="AE107" s="8"/>
+      <c r="AF107" s="8"/>
+      <c r="AG107" s="8"/>
+      <c r="AH107" s="8"/>
     </row>
     <row r="108" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -10241,10 +10179,10 @@
       <c r="AD108" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE108" s="11"/>
-      <c r="AF108" s="11"/>
-      <c r="AG108" s="11"/>
-      <c r="AH108" s="11"/>
+      <c r="AE108" s="8"/>
+      <c r="AF108" s="8"/>
+      <c r="AG108" s="8"/>
+      <c r="AH108" s="8"/>
     </row>
     <row r="109" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
@@ -10334,10 +10272,10 @@
       <c r="AD109" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE109" s="11"/>
-      <c r="AF109" s="11"/>
-      <c r="AG109" s="11"/>
-      <c r="AH109" s="11"/>
+      <c r="AE109" s="8"/>
+      <c r="AF109" s="8"/>
+      <c r="AG109" s="8"/>
+      <c r="AH109" s="8"/>
     </row>
     <row r="110" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
@@ -10427,10 +10365,10 @@
       <c r="AD110" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE110" s="11"/>
-      <c r="AF110" s="11"/>
-      <c r="AG110" s="11"/>
-      <c r="AH110" s="11"/>
+      <c r="AE110" s="8"/>
+      <c r="AF110" s="8"/>
+      <c r="AG110" s="8"/>
+      <c r="AH110" s="8"/>
     </row>
     <row r="111" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
@@ -10520,10 +10458,10 @@
       <c r="AD111" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE111" s="11"/>
-      <c r="AF111" s="11"/>
-      <c r="AG111" s="11"/>
-      <c r="AH111" s="11"/>
+      <c r="AE111" s="8"/>
+      <c r="AF111" s="8"/>
+      <c r="AG111" s="8"/>
+      <c r="AH111" s="8"/>
     </row>
     <row r="112" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
@@ -10613,10 +10551,10 @@
       <c r="AD112" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE112" s="11"/>
-      <c r="AF112" s="11"/>
-      <c r="AG112" s="11"/>
-      <c r="AH112" s="11"/>
+      <c r="AE112" s="8"/>
+      <c r="AF112" s="8"/>
+      <c r="AG112" s="8"/>
+      <c r="AH112" s="8"/>
     </row>
     <row r="113" spans="2:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
@@ -10706,10 +10644,10 @@
       <c r="AD113" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE113" s="11"/>
-      <c r="AF113" s="11"/>
-      <c r="AG113" s="11"/>
-      <c r="AH113" s="11"/>
+      <c r="AE113" s="8"/>
+      <c r="AF113" s="8"/>
+      <c r="AG113" s="8"/>
+      <c r="AH113" s="8"/>
     </row>
     <row r="114" spans="2:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
@@ -10799,10 +10737,10 @@
       <c r="AD114" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE114" s="11"/>
-      <c r="AF114" s="11"/>
-      <c r="AG114" s="11"/>
-      <c r="AH114" s="11"/>
+      <c r="AE114" s="8"/>
+      <c r="AF114" s="8"/>
+      <c r="AG114" s="8"/>
+      <c r="AH114" s="8"/>
     </row>
     <row r="115" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B115" s="2" t="s">

</xml_diff>